<commit_message>
Rint3 sur Super = 100R
</commit_message>
<xml_diff>
--- a/_Hard/_PORTS.xlsx
+++ b/_Hard/_PORTS.xlsx
@@ -505,7 +505,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="239">
   <si>
     <t>CARTE</t>
   </si>
@@ -1779,7 +1779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1955,10 +1955,52 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1976,30 +2018,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2007,21 +2025,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2321,7 +2324,7 @@
   <dimension ref="A1:AE93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18:H18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2364,45 +2367,45 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="61" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="61" t="s">
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="61" t="s">
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="61" t="s">
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="63"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="76"/>
+      <c r="AE2" s="77"/>
     </row>
     <row r="3" spans="2:31" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -2506,20 +2509,20 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
-      <c r="G4" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="65"/>
+      <c r="G4" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="79"/>
       <c r="I4" s="27" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
-      <c r="M4" s="64" t="s">
+      <c r="M4" s="78" t="s">
         <v>166</v>
       </c>
-      <c r="N4" s="65"/>
+      <c r="N4" s="79"/>
       <c r="O4" s="27" t="s">
         <v>20</v>
       </c>
@@ -2538,10 +2541,10 @@
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
       <c r="X4" s="22"/>
-      <c r="Y4" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z4" s="69"/>
+      <c r="Y4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z4" s="64"/>
       <c r="AA4" s="27" t="s">
         <v>19</v>
       </c>
@@ -2559,8 +2562,8 @@
       <c r="C5" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
+      <c r="D5" s="61">
+        <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
@@ -2568,10 +2571,10 @@
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="H5" s="69"/>
+      <c r="H5" s="64"/>
       <c r="I5" s="11" t="s">
         <v>19</v>
       </c>
@@ -2584,10 +2587,10 @@
       <c r="L5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="68" t="s">
+      <c r="M5" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="N5" s="69"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2612,10 +2615,10 @@
       <c r="X5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z5" s="69"/>
+      <c r="Y5" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="64"/>
       <c r="AA5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2648,10 +2651,10 @@
       <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="69"/>
+      <c r="G6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="64"/>
       <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
@@ -2664,10 +2667,10 @@
       <c r="L6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="68" t="s">
+      <c r="M6" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="N6" s="69"/>
+      <c r="N6" s="64"/>
       <c r="O6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2692,10 +2695,10 @@
       <c r="X6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="69"/>
+      <c r="Y6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="64"/>
       <c r="AA6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2720,10 +2723,10 @@
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="68" t="s">
+      <c r="G7" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="H7" s="69"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="11" t="s">
         <v>19</v>
       </c>
@@ -2732,10 +2735,10 @@
       <c r="L7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="68" t="s">
+      <c r="M7" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="N7" s="69"/>
+      <c r="N7" s="64"/>
       <c r="O7" s="11" t="s">
         <v>19</v>
       </c>
@@ -2758,10 +2761,10 @@
       <c r="X7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z7" s="69"/>
+      <c r="Y7" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="64"/>
       <c r="AA7" s="11" t="s">
         <v>20</v>
       </c>
@@ -2786,10 +2789,10 @@
       <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="63" t="s">
         <v>229</v>
       </c>
-      <c r="H8" s="69"/>
+      <c r="H8" s="64"/>
       <c r="I8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2798,10 +2801,10 @@
       <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="68" t="s">
+      <c r="M8" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="N8" s="69"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2824,10 +2827,10 @@
       <c r="X8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y8" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z8" s="69"/>
+      <c r="Y8" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z8" s="64"/>
       <c r="AA8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2850,20 +2853,20 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="H9" s="60"/>
+      <c r="H9" s="68"/>
       <c r="I9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="59" t="s">
+      <c r="M9" s="67" t="s">
         <v>225</v>
       </c>
-      <c r="N9" s="60"/>
+      <c r="N9" s="68"/>
       <c r="O9" s="11" t="s">
         <v>20</v>
       </c>
@@ -2882,10 +2885,10 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
-      <c r="Y9" s="68" t="s">
+      <c r="Y9" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="Z9" s="69"/>
+      <c r="Z9" s="64"/>
       <c r="AA9" s="24" t="s">
         <v>20</v>
       </c>
@@ -2906,20 +2909,20 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="67" t="s">
         <v>222</v>
       </c>
-      <c r="H10" s="60"/>
+      <c r="H10" s="68"/>
       <c r="I10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="59" t="s">
+      <c r="M10" s="67" t="s">
         <v>226</v>
       </c>
-      <c r="N10" s="60"/>
+      <c r="N10" s="68"/>
       <c r="O10" s="11" t="s">
         <v>20</v>
       </c>
@@ -2938,10 +2941,10 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="68" t="s">
+      <c r="Y10" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="Z10" s="69"/>
+      <c r="Z10" s="64"/>
       <c r="AA10" s="11" t="s">
         <v>21</v>
       </c>
@@ -2962,20 +2965,20 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="69"/>
+      <c r="G11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="64"/>
       <c r="I11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="59" t="s">
+      <c r="M11" s="67" t="s">
         <v>227</v>
       </c>
-      <c r="N11" s="60"/>
+      <c r="N11" s="68"/>
       <c r="O11" s="11" t="s">
         <v>20</v>
       </c>
@@ -2994,10 +2997,10 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="68" t="s">
+      <c r="Y11" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="Z11" s="69"/>
+      <c r="Z11" s="64"/>
       <c r="AA11" s="11" t="s">
         <v>20</v>
       </c>
@@ -3018,20 +3021,20 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="69"/>
+      <c r="G12" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="64"/>
       <c r="I12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="59" t="s">
+      <c r="M12" s="67" t="s">
         <v>224</v>
       </c>
-      <c r="N12" s="60"/>
+      <c r="N12" s="68"/>
       <c r="O12" s="11" t="s">
         <v>20</v>
       </c>
@@ -3050,10 +3053,10 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="68" t="s">
+      <c r="Y12" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="Z12" s="69"/>
+      <c r="Z12" s="64"/>
       <c r="AA12" s="11" t="s">
         <v>21</v>
       </c>
@@ -3077,7 +3080,7 @@
       <c r="G13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="81" t="s">
+      <c r="H13" s="62" t="s">
         <v>19</v>
       </c>
       <c r="I13" s="11" t="s">
@@ -3086,10 +3089,10 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="59" t="s">
+      <c r="M13" s="67" t="s">
         <v>223</v>
       </c>
-      <c r="N13" s="60"/>
+      <c r="N13" s="68"/>
       <c r="O13" s="11" t="s">
         <v>20</v>
       </c>
@@ -3108,10 +3111,10 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z13" s="69"/>
+      <c r="Y13" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z13" s="64"/>
       <c r="AA13" s="11" t="s">
         <v>20</v>
       </c>
@@ -3132,10 +3135,10 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="79" t="s">
+      <c r="G14" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="59" t="s">
         <v>237</v>
       </c>
       <c r="I14" s="24" t="s">
@@ -3144,10 +3147,10 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="79" t="s">
+      <c r="M14" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="N14" s="78" t="s">
+      <c r="N14" s="59" t="s">
         <v>237</v>
       </c>
       <c r="O14" s="11" t="s">
@@ -3168,10 +3171,10 @@
       <c r="V14" s="4"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
-      <c r="Y14" s="79" t="s">
+      <c r="Y14" s="60" t="s">
         <v>238</v>
       </c>
-      <c r="Z14" s="78" t="s">
+      <c r="Z14" s="59" t="s">
         <v>237</v>
       </c>
       <c r="AA14" s="11" t="s">
@@ -3194,20 +3197,20 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="77"/>
+      <c r="G15" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="70"/>
       <c r="I15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="59" t="s">
+      <c r="M15" s="67" t="s">
         <v>228</v>
       </c>
-      <c r="N15" s="60"/>
+      <c r="N15" s="68"/>
       <c r="O15" s="11" t="s">
         <v>20</v>
       </c>
@@ -3226,10 +3229,10 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z15" s="69"/>
+      <c r="Y15" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z15" s="64"/>
       <c r="AA15" s="11" t="s">
         <v>20</v>
       </c>
@@ -3253,7 +3256,7 @@
       <c r="G16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="78" t="s">
+      <c r="H16" s="59" t="s">
         <v>236</v>
       </c>
       <c r="I16" s="24" t="s">
@@ -3265,7 +3268,7 @@
       <c r="M16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="78" t="s">
+      <c r="N16" s="59" t="s">
         <v>236</v>
       </c>
       <c r="O16" s="11" t="s">
@@ -3289,7 +3292,7 @@
       <c r="Y16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Z16" s="78" t="s">
+      <c r="Z16" s="59" t="s">
         <v>236</v>
       </c>
       <c r="AA16" s="11" t="s">
@@ -3312,20 +3315,20 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="68" t="s">
+      <c r="G17" s="63" t="s">
         <v>231</v>
       </c>
-      <c r="H17" s="69"/>
+      <c r="H17" s="64"/>
       <c r="I17" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="66" t="s">
+      <c r="M17" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="N17" s="67"/>
+      <c r="N17" s="74"/>
       <c r="O17" s="11" t="s">
         <v>19</v>
       </c>
@@ -3344,10 +3347,10 @@
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
-      <c r="Y17" s="68" t="s">
+      <c r="Y17" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="Z17" s="69"/>
+      <c r="Z17" s="64"/>
       <c r="AA17" s="24" t="s">
         <v>20</v>
       </c>
@@ -3368,40 +3371,40 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="H18" s="69"/>
+      <c r="H18" s="64"/>
       <c r="I18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="66" t="s">
+      <c r="M18" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="67"/>
+      <c r="N18" s="74"/>
       <c r="O18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="68" t="s">
+      <c r="S18" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="T18" s="69"/>
+      <c r="T18" s="64"/>
       <c r="U18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
-      <c r="Y18" s="68" t="s">
+      <c r="Y18" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="Z18" s="69"/>
+      <c r="Z18" s="64"/>
       <c r="AA18" s="24" t="s">
         <v>20</v>
       </c>
@@ -3422,40 +3425,40 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="68" t="s">
+      <c r="G19" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="H19" s="69"/>
+      <c r="H19" s="64"/>
       <c r="I19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="66" t="s">
+      <c r="M19" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="N19" s="67"/>
+      <c r="N19" s="74"/>
       <c r="O19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="66" t="s">
+      <c r="S19" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="T19" s="67"/>
+      <c r="T19" s="74"/>
       <c r="U19" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="68" t="s">
+      <c r="Y19" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="Z19" s="69"/>
+      <c r="Z19" s="64"/>
       <c r="AA19" s="24" t="s">
         <v>20</v>
       </c>
@@ -3476,40 +3479,40 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="68" t="s">
+      <c r="G20" s="63" t="s">
         <v>234</v>
       </c>
-      <c r="H20" s="69"/>
+      <c r="H20" s="64"/>
       <c r="I20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="68" t="s">
+      <c r="M20" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="N20" s="69"/>
+      <c r="N20" s="64"/>
       <c r="O20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="68" t="s">
+      <c r="S20" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="T20" s="69"/>
+      <c r="T20" s="64"/>
       <c r="U20" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
-      <c r="Y20" s="68" t="s">
+      <c r="Y20" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="Z20" s="69"/>
+      <c r="Z20" s="64"/>
       <c r="AA20" s="24" t="s">
         <v>20</v>
       </c>
@@ -3536,10 +3539,10 @@
       <c r="F21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="68" t="s">
+      <c r="G21" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="69"/>
+      <c r="H21" s="64"/>
       <c r="I21" s="11" t="s">
         <v>19</v>
       </c>
@@ -3588,10 +3591,10 @@
       <c r="X21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y21" s="68" t="s">
+      <c r="Y21" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="Z21" s="69"/>
+      <c r="Z21" s="64"/>
       <c r="AA21" s="24" t="s">
         <v>21</v>
       </c>
@@ -3624,10 +3627,10 @@
       <c r="F22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="69"/>
+      <c r="H22" s="64"/>
       <c r="I22" s="11" t="s">
         <v>19</v>
       </c>
@@ -3676,10 +3679,10 @@
       <c r="X22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y22" s="68" t="s">
+      <c r="Y22" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="Z22" s="69"/>
+      <c r="Z22" s="64"/>
       <c r="AA22" s="24" t="s">
         <v>21</v>
       </c>
@@ -3712,10 +3715,10 @@
       <c r="F23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="68" t="s">
+      <c r="G23" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="69"/>
+      <c r="H23" s="64"/>
       <c r="I23" s="11" t="s">
         <v>21</v>
       </c>
@@ -3752,10 +3755,10 @@
       <c r="X23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y23" s="68" t="s">
+      <c r="Y23" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="Z23" s="69"/>
+      <c r="Z23" s="64"/>
       <c r="AA23" s="24" t="s">
         <v>21</v>
       </c>
@@ -3788,10 +3791,10 @@
       <c r="F24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="68" t="s">
+      <c r="G24" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="69"/>
+      <c r="H24" s="64"/>
       <c r="I24" s="11" t="s">
         <v>21</v>
       </c>
@@ -3830,10 +3833,10 @@
       <c r="X24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y24" s="68" t="s">
+      <c r="Y24" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="Z24" s="69"/>
+      <c r="Z24" s="64"/>
       <c r="AA24" s="24" t="s">
         <v>21</v>
       </c>
@@ -3866,10 +3869,10 @@
       <c r="F25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="69"/>
+      <c r="G25" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="64"/>
       <c r="I25" s="23" t="s">
         <v>21</v>
       </c>
@@ -3916,10 +3919,10 @@
       <c r="X25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Y25" s="68" t="s">
+      <c r="Y25" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="Z25" s="69"/>
+      <c r="Z25" s="64"/>
       <c r="AA25" s="25" t="s">
         <v>21</v>
       </c>
@@ -3952,10 +3955,10 @@
       <c r="F26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="69"/>
+      <c r="G26" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="64"/>
       <c r="I26" s="11" t="s">
         <v>21</v>
       </c>
@@ -4004,10 +4007,10 @@
       <c r="X26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y26" s="68" t="s">
+      <c r="Y26" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="Z26" s="69"/>
+      <c r="Z26" s="64"/>
       <c r="AA26" s="24" t="s">
         <v>21</v>
       </c>
@@ -4040,10 +4043,10 @@
       <c r="F27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="68" t="s">
+      <c r="G27" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="69"/>
+      <c r="H27" s="64"/>
       <c r="I27" s="11" t="s">
         <v>21</v>
       </c>
@@ -4092,10 +4095,10 @@
       <c r="X27" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y27" s="68" t="s">
+      <c r="Y27" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="Z27" s="69"/>
+      <c r="Z27" s="64"/>
       <c r="AA27" s="24" t="s">
         <v>21</v>
       </c>
@@ -4128,10 +4131,10 @@
       <c r="F28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="68" t="s">
+      <c r="G28" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="69"/>
+      <c r="H28" s="64"/>
       <c r="I28" s="11" t="s">
         <v>21</v>
       </c>
@@ -4180,10 +4183,10 @@
       <c r="X28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y28" s="68" t="s">
+      <c r="Y28" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="Z28" s="69"/>
+      <c r="Z28" s="64"/>
       <c r="AA28" s="24" t="s">
         <v>21</v>
       </c>
@@ -4216,10 +4219,10 @@
       <c r="F29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="68" t="s">
+      <c r="G29" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="69"/>
+      <c r="H29" s="64"/>
       <c r="I29" s="11" t="s">
         <v>21</v>
       </c>
@@ -4266,10 +4269,10 @@
       <c r="X29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y29" s="68" t="s">
+      <c r="Y29" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="Z29" s="69"/>
+      <c r="Z29" s="64"/>
       <c r="AA29" s="24" t="s">
         <v>21</v>
       </c>
@@ -4302,10 +4305,10 @@
       <c r="F30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="68" t="s">
+      <c r="G30" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="69"/>
+      <c r="H30" s="64"/>
       <c r="I30" s="11" t="s">
         <v>21</v>
       </c>
@@ -4354,10 +4357,10 @@
       <c r="X30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y30" s="68" t="s">
+      <c r="Y30" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="69"/>
+      <c r="Z30" s="64"/>
       <c r="AA30" s="24" t="s">
         <v>21</v>
       </c>
@@ -4390,10 +4393,10 @@
       <c r="F31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="68" t="s">
+      <c r="G31" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="69"/>
+      <c r="H31" s="64"/>
       <c r="I31" s="11" t="s">
         <v>21</v>
       </c>
@@ -4442,10 +4445,10 @@
       <c r="X31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y31" s="68" t="s">
+      <c r="Y31" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="Z31" s="69"/>
+      <c r="Z31" s="64"/>
       <c r="AA31" s="24" t="s">
         <v>21</v>
       </c>
@@ -4478,10 +4481,10 @@
       <c r="F32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="68" t="s">
+      <c r="G32" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="69"/>
+      <c r="H32" s="64"/>
       <c r="I32" s="11" t="s">
         <v>21</v>
       </c>
@@ -4530,10 +4533,10 @@
       <c r="X32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y32" s="68" t="s">
+      <c r="Y32" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="Z32" s="69"/>
+      <c r="Z32" s="64"/>
       <c r="AA32" s="24" t="s">
         <v>21</v>
       </c>
@@ -4566,10 +4569,10 @@
       <c r="F33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="68" t="s">
+      <c r="G33" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="69"/>
+      <c r="H33" s="64"/>
       <c r="I33" s="11" t="s">
         <v>21</v>
       </c>
@@ -4616,10 +4619,10 @@
       <c r="X33" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y33" s="68" t="s">
+      <c r="Y33" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="Z33" s="69"/>
+      <c r="Z33" s="64"/>
       <c r="AA33" s="24" t="s">
         <v>21</v>
       </c>
@@ -4652,10 +4655,10 @@
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="69"/>
+      <c r="H34" s="64"/>
       <c r="I34" s="11" t="s">
         <v>21</v>
       </c>
@@ -4704,10 +4707,10 @@
       <c r="X34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y34" s="68" t="s">
+      <c r="Y34" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="Z34" s="69"/>
+      <c r="Z34" s="64"/>
       <c r="AA34" s="24" t="s">
         <v>21</v>
       </c>
@@ -4736,10 +4739,10 @@
       <c r="F35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="68" t="s">
+      <c r="G35" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="H35" s="69"/>
+      <c r="H35" s="64"/>
       <c r="I35" s="24" t="s">
         <v>21</v>
       </c>
@@ -4748,10 +4751,10 @@
       <c r="L35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M35" s="68" t="s">
+      <c r="M35" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="N35" s="69"/>
+      <c r="N35" s="64"/>
       <c r="O35" s="24" t="s">
         <v>21</v>
       </c>
@@ -4772,10 +4775,10 @@
       <c r="X35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y35" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z35" s="69"/>
+      <c r="Y35" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z35" s="64"/>
       <c r="AA35" s="11"/>
       <c r="AB35" s="4"/>
       <c r="AC35" s="4"/>
@@ -4798,10 +4801,10 @@
       <c r="F36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="72" t="s">
+      <c r="G36" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="H36" s="73"/>
+      <c r="H36" s="66"/>
       <c r="I36" s="26" t="s">
         <v>20</v>
       </c>
@@ -4810,10 +4813,10 @@
       <c r="L36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M36" s="72" t="s">
+      <c r="M36" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="N36" s="73"/>
+      <c r="N36" s="66"/>
       <c r="O36" s="26" t="s">
         <v>20</v>
       </c>
@@ -4834,10 +4837,10 @@
       <c r="X36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Y36" s="72" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z36" s="73"/>
+      <c r="Y36" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z36" s="66"/>
       <c r="AA36" s="12"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
@@ -4972,10 +4975,10 @@
       <c r="L39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M39" s="70" t="s">
+      <c r="M39" s="71" t="s">
         <v>157</v>
       </c>
-      <c r="N39" s="71"/>
+      <c r="N39" s="72"/>
       <c r="O39" s="24" t="s">
         <v>21</v>
       </c>
@@ -5056,10 +5059,10 @@
       <c r="L40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M40" s="70" t="s">
+      <c r="M40" s="71" t="s">
         <v>155</v>
       </c>
-      <c r="N40" s="71"/>
+      <c r="N40" s="72"/>
       <c r="O40" s="24" t="s">
         <v>21</v>
       </c>
@@ -5812,68 +5815,18 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="U2:Z2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:T2"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
@@ -5887,19 +5840,69 @@
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="U2:Z2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y11:Z11"/>
     <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y20:Z20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5951,41 +5954,41 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="61" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="61" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="61" t="s">
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="62"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="61" t="s">
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="63"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="77"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -8301,34 +8304,34 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="61" t="s">
+      <c r="C2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="61" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="61" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="74" t="s">
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="76"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="82"/>
     </row>
     <row r="3" spans="2:22" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">

</xml_diff>

<commit_message>
Màj du rôle des switchs de la super.
</commit_message>
<xml_diff>
--- a/_Hard/_PORTS.xlsx
+++ b/_Hard/_PORTS.xlsx
@@ -35,6 +35,37 @@
           <t>Samuel:
 s = série
 t = tirage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Samuel Poiraud:
+XBEE ON : QS_can_over_xbee assure la connaissance du réseau XBEE, et permet l'envoi des messages sont le SID est conforme au filtre XBEE_FILTER.
+Si XBEE = OFF, les messages CAN re_us sont transmis en brut, si le mode DEBUG est activé.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Samuel Poiraud:
+L'enregistrement des messages dans l'EEPROM (après un BROADCAST_START) est conditionné à ce switch.</t>
         </r>
       </text>
     </comment>
@@ -350,11 +381,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Samuel Poiraud:
-Echo des réception 
-U1&lt;-&gt;U2
-ON / OFF
-</t>
+          <t>Samuel Poiraud:
+Les messages envoyés vers l'UART1 sont soit en VERBOSE, soit en brut.
+La réception est toujours en brut.</t>
         </r>
       </text>
     </comment>
@@ -369,7 +398,7 @@
             <family val="2"/>
           </rPr>
           <t>Samuel Poiraud:
-Echo du CAN vers U1TX</t>
+Mode DEBUG permettant un envoi vers U1 et vers U2 (Si Xbee OFF) des messages reçus.</t>
         </r>
       </text>
     </comment>
@@ -960,15 +989,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>CAN&lt;-&gt;Xbee</t>
-  </si>
-  <si>
-    <t>Echo U1&lt;-&gt;U2</t>
-  </si>
-  <si>
-    <t>CAN-&gt;U1</t>
-  </si>
-  <si>
     <t>send match</t>
   </si>
   <si>
@@ -1222,13 +1242,22 @@
   </si>
   <si>
     <t>10k vers GND</t>
+  </si>
+  <si>
+    <t>Xbee ON/OFF</t>
+  </si>
+  <si>
+    <t>VERBOSE U1</t>
+  </si>
+  <si>
+    <t>DEBUG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1257,6 +1286,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1967,40 +2003,22 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2012,10 +2030,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2323,8 +2359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2367,45 +2403,45 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="77"/>
-      <c r="I2" s="75" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="76"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="75" t="s">
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="76"/>
-      <c r="S2" s="76"/>
-      <c r="T2" s="77"/>
-      <c r="U2" s="75" t="s">
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="71"/>
+      <c r="U2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="Z2" s="77"/>
-      <c r="AA2" s="75" t="s">
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="71"/>
+      <c r="AA2" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="AB2" s="76"/>
-      <c r="AC2" s="76"/>
-      <c r="AD2" s="76"/>
-      <c r="AE2" s="77"/>
+      <c r="AB2" s="70"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="2:31" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -2424,10 +2460,10 @@
         <v>33</v>
       </c>
       <c r="G3" s="39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H3" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>32</v>
@@ -2442,10 +2478,10 @@
         <v>33</v>
       </c>
       <c r="M3" s="39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="O3" s="29" t="s">
         <v>32</v>
@@ -2460,10 +2496,10 @@
         <v>33</v>
       </c>
       <c r="S3" s="39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="T3" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="U3" s="29" t="s">
         <v>32</v>
@@ -2478,10 +2514,10 @@
         <v>33</v>
       </c>
       <c r="Y3" s="39" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="Z3" s="58" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="AA3" s="29" t="s">
         <v>32</v>
@@ -2509,20 +2545,20 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
-      <c r="G4" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="79"/>
+      <c r="G4" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="66"/>
       <c r="I4" s="27" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
-      <c r="M4" s="78" t="s">
-        <v>166</v>
-      </c>
-      <c r="N4" s="79"/>
+      <c r="M4" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="N4" s="66"/>
       <c r="O4" s="27" t="s">
         <v>20</v>
       </c>
@@ -2541,10 +2577,10 @@
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
       <c r="X4" s="22"/>
-      <c r="Y4" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z4" s="64"/>
+      <c r="Y4" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z4" s="68"/>
       <c r="AA4" s="27" t="s">
         <v>19</v>
       </c>
@@ -2571,10 +2607,10 @@
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="63" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="64"/>
+      <c r="G5" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="68"/>
       <c r="I5" s="11" t="s">
         <v>19</v>
       </c>
@@ -2587,10 +2623,10 @@
       <c r="L5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="N5" s="64"/>
+      <c r="M5" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="N5" s="68"/>
       <c r="O5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2615,10 +2651,10 @@
       <c r="X5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z5" s="64"/>
+      <c r="Y5" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="68"/>
       <c r="AA5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2651,10 +2687,10 @@
       <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="64"/>
+      <c r="G6" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="68"/>
       <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
@@ -2667,10 +2703,10 @@
       <c r="L6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="N6" s="64"/>
+      <c r="M6" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="N6" s="68"/>
       <c r="O6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2695,10 +2731,10 @@
       <c r="X6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="64"/>
+      <c r="Y6" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="68"/>
       <c r="AA6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2716,17 +2752,17 @@
         <v>44</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="63" t="s">
-        <v>230</v>
-      </c>
-      <c r="H7" s="64"/>
+      <c r="G7" s="67" t="s">
+        <v>227</v>
+      </c>
+      <c r="H7" s="68"/>
       <c r="I7" s="11" t="s">
         <v>19</v>
       </c>
@@ -2735,10 +2771,10 @@
       <c r="L7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="N7" s="64"/>
+      <c r="M7" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="N7" s="68"/>
       <c r="O7" s="11" t="s">
         <v>19</v>
       </c>
@@ -2761,10 +2797,10 @@
       <c r="X7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z7" s="64"/>
+      <c r="Y7" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="68"/>
       <c r="AA7" s="11" t="s">
         <v>20</v>
       </c>
@@ -2782,17 +2818,17 @@
         <v>45</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="63" t="s">
-        <v>229</v>
-      </c>
-      <c r="H8" s="64"/>
+      <c r="G8" s="67" t="s">
+        <v>226</v>
+      </c>
+      <c r="H8" s="68"/>
       <c r="I8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2801,10 +2837,10 @@
       <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="N8" s="64"/>
+      <c r="M8" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="N8" s="68"/>
       <c r="O8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2827,10 +2863,10 @@
       <c r="X8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y8" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z8" s="64"/>
+      <c r="Y8" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z8" s="68"/>
       <c r="AA8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2853,20 +2889,20 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="67" t="s">
-        <v>151</v>
-      </c>
-      <c r="H9" s="68"/>
+      <c r="G9" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="H9" s="64"/>
       <c r="I9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="67" t="s">
-        <v>225</v>
-      </c>
-      <c r="N9" s="68"/>
+      <c r="M9" s="63" t="s">
+        <v>222</v>
+      </c>
+      <c r="N9" s="64"/>
       <c r="O9" s="11" t="s">
         <v>20</v>
       </c>
@@ -2874,10 +2910,10 @@
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
       <c r="S9" s="49" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="T9" s="50" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="U9" s="24" t="s">
         <v>20</v>
@@ -2885,10 +2921,10 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
-      <c r="Y9" s="63" t="s">
+      <c r="Y9" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="Z9" s="64"/>
+      <c r="Z9" s="68"/>
       <c r="AA9" s="24" t="s">
         <v>20</v>
       </c>
@@ -2909,20 +2945,20 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="67" t="s">
-        <v>222</v>
-      </c>
-      <c r="H10" s="68"/>
+      <c r="G10" s="63" t="s">
+        <v>219</v>
+      </c>
+      <c r="H10" s="64"/>
       <c r="I10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="67" t="s">
-        <v>226</v>
-      </c>
-      <c r="N10" s="68"/>
+      <c r="M10" s="63" t="s">
+        <v>223</v>
+      </c>
+      <c r="N10" s="64"/>
       <c r="O10" s="11" t="s">
         <v>20</v>
       </c>
@@ -2930,10 +2966,10 @@
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
       <c r="S10" s="49" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="T10" s="50" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="U10" s="24" t="s">
         <v>20</v>
@@ -2941,10 +2977,10 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="63" t="s">
+      <c r="Y10" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="Z10" s="64"/>
+      <c r="Z10" s="68"/>
       <c r="AA10" s="11" t="s">
         <v>21</v>
       </c>
@@ -2965,20 +3001,20 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="64"/>
+      <c r="G11" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="68"/>
       <c r="I11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="67" t="s">
-        <v>227</v>
-      </c>
-      <c r="N11" s="68"/>
+      <c r="M11" s="63" t="s">
+        <v>224</v>
+      </c>
+      <c r="N11" s="64"/>
       <c r="O11" s="11" t="s">
         <v>20</v>
       </c>
@@ -2986,7 +3022,7 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
       <c r="S11" s="49" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="T11" s="10" t="s">
         <v>19</v>
@@ -2997,10 +3033,10 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="63" t="s">
+      <c r="Y11" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="Z11" s="64"/>
+      <c r="Z11" s="68"/>
       <c r="AA11" s="11" t="s">
         <v>20</v>
       </c>
@@ -3021,20 +3057,20 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="64"/>
+      <c r="G12" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="68"/>
       <c r="I12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="67" t="s">
-        <v>224</v>
-      </c>
-      <c r="N12" s="68"/>
+      <c r="M12" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="N12" s="64"/>
       <c r="O12" s="11" t="s">
         <v>20</v>
       </c>
@@ -3042,7 +3078,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="49" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="T12" s="10" t="s">
         <v>19</v>
@@ -3053,10 +3089,10 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="63" t="s">
+      <c r="Y12" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="Z12" s="64"/>
+      <c r="Z12" s="68"/>
       <c r="AA12" s="11" t="s">
         <v>21</v>
       </c>
@@ -3089,10 +3125,10 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="67" t="s">
-        <v>223</v>
-      </c>
-      <c r="N13" s="68"/>
+      <c r="M13" s="63" t="s">
+        <v>220</v>
+      </c>
+      <c r="N13" s="64"/>
       <c r="O13" s="11" t="s">
         <v>20</v>
       </c>
@@ -3100,7 +3136,7 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
       <c r="S13" s="49" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="T13" s="10" t="s">
         <v>19</v>
@@ -3111,10 +3147,10 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z13" s="64"/>
+      <c r="Y13" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z13" s="68"/>
       <c r="AA13" s="11" t="s">
         <v>20</v>
       </c>
@@ -3136,10 +3172,10 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="60" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H14" s="59" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>21</v>
@@ -3148,10 +3184,10 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="60" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N14" s="59" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="O14" s="11" t="s">
         <v>20</v>
@@ -3160,7 +3196,7 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="49" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="T14" s="10" t="s">
         <v>19</v>
@@ -3172,10 +3208,10 @@
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="60" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="Z14" s="59" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="AA14" s="11" t="s">
         <v>21</v>
@@ -3197,20 +3233,20 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="69" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="70"/>
+      <c r="G15" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="79"/>
       <c r="I15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="67" t="s">
-        <v>228</v>
-      </c>
-      <c r="N15" s="68"/>
+      <c r="M15" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="N15" s="64"/>
       <c r="O15" s="11" t="s">
         <v>20</v>
       </c>
@@ -3218,7 +3254,7 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="49" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="T15" s="10" t="s">
         <v>19</v>
@@ -3229,10 +3265,10 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z15" s="64"/>
+      <c r="Y15" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z15" s="68"/>
       <c r="AA15" s="11" t="s">
         <v>20</v>
       </c>
@@ -3257,7 +3293,7 @@
         <v>19</v>
       </c>
       <c r="H16" s="59" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>20</v>
@@ -3269,7 +3305,7 @@
         <v>19</v>
       </c>
       <c r="N16" s="59" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="O16" s="11" t="s">
         <v>20</v>
@@ -3278,7 +3314,7 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="49" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="T16" s="10" t="s">
         <v>19</v>
@@ -3293,7 +3329,7 @@
         <v>19</v>
       </c>
       <c r="Z16" s="59" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="AA16" s="11" t="s">
         <v>21</v>
@@ -3315,20 +3351,20 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="63" t="s">
-        <v>231</v>
-      </c>
-      <c r="H17" s="64"/>
+      <c r="G17" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="H17" s="68"/>
       <c r="I17" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="73" t="s">
+      <c r="M17" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="N17" s="74"/>
+      <c r="N17" s="73"/>
       <c r="O17" s="11" t="s">
         <v>19</v>
       </c>
@@ -3336,10 +3372,10 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="49" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="T17" s="50" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="U17" s="24" t="s">
         <v>20</v>
@@ -3347,10 +3383,10 @@
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
-      <c r="Y17" s="63" t="s">
+      <c r="Y17" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="Z17" s="64"/>
+      <c r="Z17" s="68"/>
       <c r="AA17" s="24" t="s">
         <v>20</v>
       </c>
@@ -3371,40 +3407,40 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="63" t="s">
-        <v>232</v>
-      </c>
-      <c r="H18" s="64"/>
+      <c r="G18" s="67" t="s">
+        <v>229</v>
+      </c>
+      <c r="H18" s="68"/>
       <c r="I18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="73" t="s">
+      <c r="M18" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="74"/>
+      <c r="N18" s="73"/>
       <c r="O18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="T18" s="64"/>
+      <c r="S18" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="T18" s="68"/>
       <c r="U18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
-      <c r="Y18" s="63" t="s">
+      <c r="Y18" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="Z18" s="64"/>
+      <c r="Z18" s="68"/>
       <c r="AA18" s="24" t="s">
         <v>20</v>
       </c>
@@ -3425,40 +3461,40 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="63" t="s">
-        <v>233</v>
-      </c>
-      <c r="H19" s="64"/>
+      <c r="G19" s="67" t="s">
+        <v>230</v>
+      </c>
+      <c r="H19" s="68"/>
       <c r="I19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="73" t="s">
+      <c r="M19" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="N19" s="74"/>
+      <c r="N19" s="73"/>
       <c r="O19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="73" t="s">
+      <c r="S19" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="T19" s="74"/>
+      <c r="T19" s="73"/>
       <c r="U19" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="63" t="s">
+      <c r="Y19" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="Z19" s="64"/>
+      <c r="Z19" s="68"/>
       <c r="AA19" s="24" t="s">
         <v>20</v>
       </c>
@@ -3479,40 +3515,40 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="H20" s="64"/>
+      <c r="G20" s="67" t="s">
+        <v>231</v>
+      </c>
+      <c r="H20" s="68"/>
       <c r="I20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="N20" s="64"/>
+      <c r="M20" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="N20" s="68"/>
       <c r="O20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="63" t="s">
+      <c r="S20" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="T20" s="64"/>
+      <c r="T20" s="68"/>
       <c r="U20" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
-      <c r="Y20" s="63" t="s">
+      <c r="Y20" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="Z20" s="64"/>
+      <c r="Z20" s="68"/>
       <c r="AA20" s="24" t="s">
         <v>20</v>
       </c>
@@ -3539,10 +3575,10 @@
       <c r="F21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="63" t="s">
+      <c r="G21" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="64"/>
+      <c r="H21" s="68"/>
       <c r="I21" s="11" t="s">
         <v>19</v>
       </c>
@@ -3556,10 +3592,10 @@
         <v>19</v>
       </c>
       <c r="M21" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O21" s="11" t="s">
         <v>21</v>
@@ -3568,16 +3604,16 @@
         <v>76</v>
       </c>
       <c r="Q21" s="54" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="R21" s="54" t="s">
         <v>79</v>
       </c>
       <c r="S21" s="49" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="T21" s="50" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="U21" s="24" t="s">
         <v>21</v>
@@ -3591,10 +3627,10 @@
       <c r="X21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y21" s="63" t="s">
-        <v>161</v>
-      </c>
-      <c r="Z21" s="64"/>
+      <c r="Y21" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z21" s="68"/>
       <c r="AA21" s="24" t="s">
         <v>21</v>
       </c>
@@ -3627,10 +3663,10 @@
       <c r="F22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="63" t="s">
+      <c r="G22" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="64"/>
+      <c r="H22" s="68"/>
       <c r="I22" s="11" t="s">
         <v>19</v>
       </c>
@@ -3644,10 +3680,10 @@
         <v>19</v>
       </c>
       <c r="M22" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O22" s="11" t="s">
         <v>21</v>
@@ -3656,16 +3692,16 @@
         <v>76</v>
       </c>
       <c r="Q22" s="54" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="R22" s="54" t="s">
         <v>79</v>
       </c>
       <c r="S22" s="49" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="T22" s="50" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="U22" s="24" t="s">
         <v>21</v>
@@ -3679,10 +3715,10 @@
       <c r="X22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y22" s="63" t="s">
-        <v>160</v>
-      </c>
-      <c r="Z22" s="64"/>
+      <c r="Y22" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z22" s="68"/>
       <c r="AA22" s="24" t="s">
         <v>21</v>
       </c>
@@ -3715,10 +3751,10 @@
       <c r="F23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="63" t="s">
+      <c r="G23" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="64"/>
+      <c r="H23" s="68"/>
       <c r="I23" s="11" t="s">
         <v>21</v>
       </c>
@@ -3732,7 +3768,7 @@
         <v>79</v>
       </c>
       <c r="M23" s="49" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="N23" s="10"/>
       <c r="O23" s="11" t="s">
@@ -3755,10 +3791,10 @@
       <c r="X23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y23" s="63" t="s">
-        <v>159</v>
-      </c>
-      <c r="Z23" s="64"/>
+      <c r="Y23" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z23" s="68"/>
       <c r="AA23" s="24" t="s">
         <v>21</v>
       </c>
@@ -3791,10 +3827,10 @@
       <c r="F24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="G24" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="64"/>
+      <c r="H24" s="68"/>
       <c r="I24" s="11" t="s">
         <v>21</v>
       </c>
@@ -3808,10 +3844,10 @@
         <v>19</v>
       </c>
       <c r="M24" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O24" s="11" t="s">
         <v>21</v>
@@ -3833,10 +3869,10 @@
       <c r="X24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y24" s="63" t="s">
-        <v>158</v>
-      </c>
-      <c r="Z24" s="64"/>
+      <c r="Y24" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z24" s="68"/>
       <c r="AA24" s="24" t="s">
         <v>21</v>
       </c>
@@ -3869,10 +3905,10 @@
       <c r="F25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="64"/>
+      <c r="G25" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="68"/>
       <c r="I25" s="23" t="s">
         <v>21</v>
       </c>
@@ -3886,7 +3922,7 @@
         <v>79</v>
       </c>
       <c r="M25" s="49" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="N25" s="46"/>
       <c r="O25" s="23" t="s">
@@ -3902,10 +3938,10 @@
         <v>19</v>
       </c>
       <c r="S25" s="49" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="T25" s="50" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="U25" s="25" t="s">
         <v>21</v>
@@ -3919,10 +3955,10 @@
       <c r="X25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Y25" s="63" t="s">
+      <c r="Y25" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="Z25" s="64"/>
+      <c r="Z25" s="68"/>
       <c r="AA25" s="25" t="s">
         <v>21</v>
       </c>
@@ -3955,10 +3991,10 @@
       <c r="F26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="64"/>
+      <c r="G26" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="68"/>
       <c r="I26" s="11" t="s">
         <v>21</v>
       </c>
@@ -3972,10 +4008,10 @@
         <v>19</v>
       </c>
       <c r="M26" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O26" s="11" t="s">
         <v>21</v>
@@ -3990,10 +4026,10 @@
         <v>19</v>
       </c>
       <c r="S26" s="49" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="T26" s="50" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="U26" s="24" t="s">
         <v>21</v>
@@ -4007,10 +4043,10 @@
       <c r="X26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y26" s="63" t="s">
+      <c r="Y26" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="Z26" s="64"/>
+      <c r="Z26" s="68"/>
       <c r="AA26" s="24" t="s">
         <v>21</v>
       </c>
@@ -4043,10 +4079,10 @@
       <c r="F27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="63" t="s">
+      <c r="G27" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="64"/>
+      <c r="H27" s="68"/>
       <c r="I27" s="11" t="s">
         <v>21</v>
       </c>
@@ -4060,10 +4096,10 @@
         <v>79</v>
       </c>
       <c r="M27" s="50" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="N27" s="50" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O27" s="11" t="s">
         <v>21</v>
@@ -4078,10 +4114,10 @@
         <v>19</v>
       </c>
       <c r="S27" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T27" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="U27" s="24" t="s">
         <v>21</v>
@@ -4095,10 +4131,10 @@
       <c r="X27" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y27" s="63" t="s">
+      <c r="Y27" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="Z27" s="64"/>
+      <c r="Z27" s="68"/>
       <c r="AA27" s="24" t="s">
         <v>21</v>
       </c>
@@ -4131,10 +4167,10 @@
       <c r="F28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="63" t="s">
+      <c r="G28" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="64"/>
+      <c r="H28" s="68"/>
       <c r="I28" s="11" t="s">
         <v>21</v>
       </c>
@@ -4148,10 +4184,10 @@
         <v>19</v>
       </c>
       <c r="M28" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O28" s="11" t="s">
         <v>21</v>
@@ -4166,10 +4202,10 @@
         <v>19</v>
       </c>
       <c r="S28" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T28" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="U28" s="24" t="s">
         <v>21</v>
@@ -4183,10 +4219,10 @@
       <c r="X28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y28" s="63" t="s">
+      <c r="Y28" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="Z28" s="64"/>
+      <c r="Z28" s="68"/>
       <c r="AA28" s="24" t="s">
         <v>21</v>
       </c>
@@ -4219,10 +4255,10 @@
       <c r="F29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="63" t="s">
+      <c r="G29" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="64"/>
+      <c r="H29" s="68"/>
       <c r="I29" s="11" t="s">
         <v>21</v>
       </c>
@@ -4236,10 +4272,10 @@
         <v>79</v>
       </c>
       <c r="M29" s="50" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="N29" s="50" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O29" s="11" t="s">
         <v>21</v>
@@ -4255,7 +4291,7 @@
       </c>
       <c r="S29" s="48"/>
       <c r="T29" s="50" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="U29" s="24" t="s">
         <v>21</v>
@@ -4269,10 +4305,10 @@
       <c r="X29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y29" s="63" t="s">
+      <c r="Y29" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="Z29" s="64"/>
+      <c r="Z29" s="68"/>
       <c r="AA29" s="24" t="s">
         <v>21</v>
       </c>
@@ -4305,10 +4341,10 @@
       <c r="F30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="63" t="s">
+      <c r="G30" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="64"/>
+      <c r="H30" s="68"/>
       <c r="I30" s="11" t="s">
         <v>21</v>
       </c>
@@ -4322,10 +4358,10 @@
         <v>19</v>
       </c>
       <c r="M30" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O30" s="11" t="s">
         <v>21</v>
@@ -4340,10 +4376,10 @@
         <v>19</v>
       </c>
       <c r="S30" s="49" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="T30" s="50" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="U30" s="24" t="s">
         <v>21</v>
@@ -4357,10 +4393,10 @@
       <c r="X30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y30" s="63" t="s">
+      <c r="Y30" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="64"/>
+      <c r="Z30" s="68"/>
       <c r="AA30" s="24" t="s">
         <v>21</v>
       </c>
@@ -4393,10 +4429,10 @@
       <c r="F31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="63" t="s">
+      <c r="G31" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="64"/>
+      <c r="H31" s="68"/>
       <c r="I31" s="11" t="s">
         <v>21</v>
       </c>
@@ -4410,10 +4446,10 @@
         <v>19</v>
       </c>
       <c r="M31" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O31" s="11" t="s">
         <v>21</v>
@@ -4428,10 +4464,10 @@
         <v>19</v>
       </c>
       <c r="S31" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T31" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="U31" s="24" t="s">
         <v>21</v>
@@ -4445,10 +4481,10 @@
       <c r="X31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y31" s="63" t="s">
+      <c r="Y31" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="Z31" s="64"/>
+      <c r="Z31" s="68"/>
       <c r="AA31" s="24" t="s">
         <v>21</v>
       </c>
@@ -4481,10 +4517,10 @@
       <c r="F32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="63" t="s">
+      <c r="G32" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="64"/>
+      <c r="H32" s="68"/>
       <c r="I32" s="11" t="s">
         <v>21</v>
       </c>
@@ -4498,10 +4534,10 @@
         <v>19</v>
       </c>
       <c r="M32" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O32" s="11" t="s">
         <v>21</v>
@@ -4516,10 +4552,10 @@
         <v>19</v>
       </c>
       <c r="S32" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="T32" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="U32" s="24" t="s">
         <v>21</v>
@@ -4533,10 +4569,10 @@
       <c r="X32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y32" s="63" t="s">
+      <c r="Y32" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="Z32" s="64"/>
+      <c r="Z32" s="68"/>
       <c r="AA32" s="24" t="s">
         <v>21</v>
       </c>
@@ -4569,10 +4605,10 @@
       <c r="F33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="63" t="s">
+      <c r="G33" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="64"/>
+      <c r="H33" s="68"/>
       <c r="I33" s="11" t="s">
         <v>21</v>
       </c>
@@ -4602,10 +4638,10 @@
         <v>19</v>
       </c>
       <c r="S33" s="49" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="T33" s="50" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="U33" s="24" t="s">
         <v>21</v>
@@ -4619,10 +4655,10 @@
       <c r="X33" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y33" s="63" t="s">
+      <c r="Y33" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="Z33" s="64"/>
+      <c r="Z33" s="68"/>
       <c r="AA33" s="24" t="s">
         <v>21</v>
       </c>
@@ -4655,10 +4691,10 @@
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="63" t="s">
+      <c r="G34" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="64"/>
+      <c r="H34" s="68"/>
       <c r="I34" s="11" t="s">
         <v>21</v>
       </c>
@@ -4672,10 +4708,10 @@
         <v>19</v>
       </c>
       <c r="M34" s="41" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="O34" s="11" t="s">
         <v>21</v>
@@ -4690,10 +4726,10 @@
         <v>79</v>
       </c>
       <c r="S34" s="49" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="T34" s="50" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="U34" s="24" t="s">
         <v>21</v>
@@ -4707,10 +4743,10 @@
       <c r="X34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y34" s="63" t="s">
+      <c r="Y34" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="Z34" s="64"/>
+      <c r="Z34" s="68"/>
       <c r="AA34" s="24" t="s">
         <v>21</v>
       </c>
@@ -4739,10 +4775,10 @@
       <c r="F35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="63" t="s">
-        <v>162</v>
-      </c>
-      <c r="H35" s="64"/>
+      <c r="G35" s="67" t="s">
+        <v>159</v>
+      </c>
+      <c r="H35" s="68"/>
       <c r="I35" s="24" t="s">
         <v>21</v>
       </c>
@@ -4751,10 +4787,10 @@
       <c r="L35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M35" s="63" t="s">
+      <c r="M35" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="N35" s="64"/>
+      <c r="N35" s="68"/>
       <c r="O35" s="24" t="s">
         <v>21</v>
       </c>
@@ -4775,10 +4811,10 @@
       <c r="X35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y35" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z35" s="64"/>
+      <c r="Y35" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z35" s="68"/>
       <c r="AA35" s="11"/>
       <c r="AB35" s="4"/>
       <c r="AC35" s="4"/>
@@ -4801,10 +4837,10 @@
       <c r="F36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="65" t="s">
-        <v>163</v>
-      </c>
-      <c r="H36" s="66"/>
+      <c r="G36" s="76" t="s">
+        <v>160</v>
+      </c>
+      <c r="H36" s="77"/>
       <c r="I36" s="26" t="s">
         <v>20</v>
       </c>
@@ -4813,10 +4849,10 @@
       <c r="L36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M36" s="65" t="s">
+      <c r="M36" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="N36" s="66"/>
+      <c r="N36" s="77"/>
       <c r="O36" s="26" t="s">
         <v>20</v>
       </c>
@@ -4837,10 +4873,10 @@
       <c r="X36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Y36" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z36" s="66"/>
+      <c r="Y36" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z36" s="77"/>
       <c r="AA36" s="12"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
@@ -4863,7 +4899,7 @@
       <c r="F37" s="22"/>
       <c r="G37" s="40"/>
       <c r="H37" s="34" t="s">
-        <v>152</v>
+        <v>237</v>
       </c>
       <c r="I37" s="33" t="s">
         <v>21</v>
@@ -4909,7 +4945,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="42"/>
       <c r="H38" s="35" t="s">
-        <v>153</v>
+        <v>238</v>
       </c>
       <c r="I38" s="24" t="s">
         <v>21</v>
@@ -4961,7 +4997,7 @@
       </c>
       <c r="G39" s="57"/>
       <c r="H39" s="36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I39" s="24" t="s">
         <v>21</v>
@@ -4975,10 +5011,10 @@
       <c r="L39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M39" s="71" t="s">
-        <v>157</v>
-      </c>
-      <c r="N39" s="72"/>
+      <c r="M39" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="N39" s="75"/>
       <c r="O39" s="24" t="s">
         <v>21</v>
       </c>
@@ -4992,10 +5028,10 @@
         <v>79</v>
       </c>
       <c r="S39" s="52" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="T39" s="36" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="U39" s="24" t="s">
         <v>21</v>
@@ -5011,7 +5047,7 @@
       </c>
       <c r="Y39" s="57"/>
       <c r="Z39" s="36" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AA39" s="24" t="s">
         <v>21</v>
@@ -5045,7 +5081,7 @@
       </c>
       <c r="G40" s="57"/>
       <c r="H40" s="36" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="I40" s="24" t="s">
         <v>21</v>
@@ -5059,10 +5095,10 @@
       <c r="L40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M40" s="71" t="s">
-        <v>155</v>
-      </c>
-      <c r="N40" s="72"/>
+      <c r="M40" s="74" t="s">
+        <v>152</v>
+      </c>
+      <c r="N40" s="75"/>
       <c r="O40" s="24" t="s">
         <v>21</v>
       </c>
@@ -5076,10 +5112,10 @@
         <v>79</v>
       </c>
       <c r="S40" s="52" t="s">
+        <v>206</v>
+      </c>
+      <c r="T40" s="36" t="s">
         <v>209</v>
-      </c>
-      <c r="T40" s="36" t="s">
-        <v>212</v>
       </c>
       <c r="U40" s="24" t="s">
         <v>21</v>
@@ -5154,10 +5190,10 @@
         <v>79</v>
       </c>
       <c r="S41" s="52" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="T41" s="36" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="U41" s="24" t="s">
         <v>21</v>
@@ -5233,10 +5269,10 @@
         <v>79</v>
       </c>
       <c r="S42" s="52" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="T42" s="36" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="U42" s="24" t="s">
         <v>21</v>
@@ -5336,7 +5372,7 @@
       <c r="F44" s="4"/>
       <c r="G44" s="42"/>
       <c r="H44" s="56" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I44" s="24" t="s">
         <v>20</v>
@@ -5348,7 +5384,7 @@
       <c r="L44" s="4"/>
       <c r="M44" s="42"/>
       <c r="N44" s="56" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="O44" s="24" t="s">
         <v>20</v>
@@ -5360,7 +5396,7 @@
       <c r="R44" s="4"/>
       <c r="S44" s="42"/>
       <c r="T44" s="56" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="U44" s="24" t="s">
         <v>20</v>
@@ -5372,7 +5408,7 @@
       <c r="X44" s="4"/>
       <c r="Y44" s="42"/>
       <c r="Z44" s="56" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AA44" s="24" t="s">
         <v>20</v>
@@ -5399,7 +5435,7 @@
       <c r="F45" s="4"/>
       <c r="G45" s="42"/>
       <c r="H45" s="56" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I45" s="24" t="s">
         <v>20</v>
@@ -5411,7 +5447,7 @@
       <c r="L45" s="4"/>
       <c r="M45" s="42"/>
       <c r="N45" s="56" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="O45" s="24" t="s">
         <v>20</v>
@@ -5423,7 +5459,7 @@
       <c r="R45" s="4"/>
       <c r="S45" s="42"/>
       <c r="T45" s="56" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="U45" s="24" t="s">
         <v>20</v>
@@ -5435,7 +5471,7 @@
       <c r="X45" s="4"/>
       <c r="Y45" s="42"/>
       <c r="Z45" s="56" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AA45" s="24" t="s">
         <v>20</v>
@@ -5623,7 +5659,7 @@
     <row r="52" spans="1:16">
       <c r="B52" s="37"/>
       <c r="M52" s="38" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -5637,7 +5673,7 @@
       <c r="H54" s="2"/>
       <c r="K54" s="37"/>
       <c r="M54" s="38" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -5645,7 +5681,7 @@
       <c r="H55" s="2"/>
       <c r="K55" s="37"/>
       <c r="M55" s="44" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -5653,7 +5689,7 @@
       <c r="H56" s="2"/>
       <c r="K56" s="37"/>
       <c r="M56" s="44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -5661,7 +5697,7 @@
       <c r="H57" s="2"/>
       <c r="K57" s="37"/>
       <c r="M57" s="44" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -5669,7 +5705,7 @@
       <c r="H58" s="38"/>
       <c r="K58" s="37"/>
       <c r="M58" s="44" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -5677,7 +5713,7 @@
       <c r="H59" s="2"/>
       <c r="K59" s="37"/>
       <c r="M59" s="44" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -5685,7 +5721,7 @@
       <c r="H60" s="2"/>
       <c r="K60" s="37"/>
       <c r="M60" s="44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -5702,7 +5738,7 @@
     <row r="63" spans="1:16">
       <c r="H63" s="2"/>
       <c r="M63" s="38" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P63" s="37"/>
     </row>
@@ -5711,7 +5747,7 @@
       <c r="H64" s="2"/>
       <c r="K64" s="38"/>
       <c r="M64" s="44" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="P64" s="37"/>
     </row>
@@ -5719,7 +5755,7 @@
       <c r="B65" s="37"/>
       <c r="H65" s="2"/>
       <c r="M65" s="37" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="P65" s="37"/>
     </row>
@@ -5815,18 +5851,68 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="U2:Z2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="M20:N20"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="M7:N7"/>
@@ -5840,69 +5926,19 @@
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S18:T18"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="U2:Z2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:T2"/>
     <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5954,41 +5990,41 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="75" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="75" t="s">
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="75" t="s">
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="76"/>
-      <c r="T2" s="76"/>
-      <c r="U2" s="76"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="75" t="s">
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="71"/>
+      <c r="W2" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
-      <c r="Z2" s="76"/>
-      <c r="AA2" s="77"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="71"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -8304,27 +8340,27 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="75" t="s">
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="75" t="s">
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="76"/>
-      <c r="O2" s="76"/>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="77"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="71"/>
       <c r="R2" s="80" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Ajout infos cablage tritronics CW-2
</commit_message>
<xml_diff>
--- a/_Hard/_PORTS.xlsx
+++ b/_Hard/_PORTS.xlsx
@@ -534,7 +534,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="262">
   <si>
     <t>CARTE</t>
   </si>
@@ -1251,13 +1251,82 @@
   </si>
   <si>
     <t>DEBUG</t>
+  </si>
+  <si>
+    <t>couleur fil      </t>
+  </si>
+  <si>
+    <t>signal capteur            </t>
+  </si>
+  <si>
+    <t>Port du dsPIC</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>RE8_INT1 (pullup 100k sur la carte)</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>RE9_INT2 (pullup 100k sur la carte)</t>
+  </si>
+  <si>
+    <t>Red/White</t>
+  </si>
+  <si>
+    <t>Analog x (rouge)  </t>
+  </si>
+  <si>
+    <t>RB13 (pas de tirage, sortie 0-5V)</t>
+  </si>
+  <si>
+    <t>Green/white</t>
+  </si>
+  <si>
+    <t>Analog y (vert)</t>
+  </si>
+  <si>
+    <t>RB12 (pas de tirage, sortie 0-5V)</t>
+  </si>
+  <si>
+    <t>Blue/white</t>
+  </si>
+  <si>
+    <t>Analog Y (VERT)</t>
+  </si>
+  <si>
+    <t>RB2 (pas de tirage, sortie 0-5V)</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>24V</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>0V</t>
+  </si>
+  <si>
+    <t>CH2 (Bleu numérique)  </t>
+  </si>
+  <si>
+    <t>CH1 (Rouge numérique)</t>
+  </si>
+  <si>
+    <t>Tritronics CW-2 (config NPN, xyY)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1293,6 +1362,28 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1345,7 +1436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1811,11 +1902,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2003,22 +2103,40 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2030,28 +2148,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2062,6 +2162,67 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2359,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="G37" workbookViewId="0">
+      <selection activeCell="S54" sqref="S54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2403,45 +2564,45 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="69" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="69" t="s">
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="69" t="s">
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="69" t="s">
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="71"/>
+      <c r="AB2" s="76"/>
+      <c r="AC2" s="76"/>
+      <c r="AD2" s="76"/>
+      <c r="AE2" s="77"/>
     </row>
     <row r="3" spans="2:31" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -2545,20 +2706,20 @@
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
-      <c r="G4" s="65" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="66"/>
+      <c r="G4" s="78" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="79"/>
       <c r="I4" s="27" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
-      <c r="M4" s="65" t="s">
+      <c r="M4" s="78" t="s">
         <v>163</v>
       </c>
-      <c r="N4" s="66"/>
+      <c r="N4" s="79"/>
       <c r="O4" s="27" t="s">
         <v>20</v>
       </c>
@@ -2577,10 +2738,10 @@
       <c r="V4" s="22"/>
       <c r="W4" s="22"/>
       <c r="X4" s="22"/>
-      <c r="Y4" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z4" s="68"/>
+      <c r="Y4" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z4" s="64"/>
       <c r="AA4" s="27" t="s">
         <v>19</v>
       </c>
@@ -2607,10 +2768,10 @@
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="67" t="s">
+      <c r="G5" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="H5" s="68"/>
+      <c r="H5" s="64"/>
       <c r="I5" s="11" t="s">
         <v>19</v>
       </c>
@@ -2623,10 +2784,10 @@
       <c r="L5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="67" t="s">
+      <c r="M5" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="N5" s="68"/>
+      <c r="N5" s="64"/>
       <c r="O5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2651,10 +2812,10 @@
       <c r="X5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y5" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z5" s="68"/>
+      <c r="Y5" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z5" s="64"/>
       <c r="AA5" s="11" t="s">
         <v>21</v>
       </c>
@@ -2687,10 +2848,10 @@
       <c r="F6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="68"/>
+      <c r="G6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="64"/>
       <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
@@ -2703,10 +2864,10 @@
       <c r="L6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="67" t="s">
+      <c r="M6" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="N6" s="68"/>
+      <c r="N6" s="64"/>
       <c r="O6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2731,10 +2892,10 @@
       <c r="X6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y6" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="68"/>
+      <c r="Y6" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="64"/>
       <c r="AA6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2759,10 +2920,10 @@
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="63" t="s">
         <v>227</v>
       </c>
-      <c r="H7" s="68"/>
+      <c r="H7" s="64"/>
       <c r="I7" s="11" t="s">
         <v>19</v>
       </c>
@@ -2771,10 +2932,10 @@
       <c r="L7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="67" t="s">
+      <c r="M7" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="N7" s="68"/>
+      <c r="N7" s="64"/>
       <c r="O7" s="11" t="s">
         <v>19</v>
       </c>
@@ -2797,10 +2958,10 @@
       <c r="X7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z7" s="68"/>
+      <c r="Y7" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="64"/>
       <c r="AA7" s="11" t="s">
         <v>20</v>
       </c>
@@ -2825,10 +2986,10 @@
       <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="67" t="s">
+      <c r="G8" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="H8" s="68"/>
+      <c r="H8" s="64"/>
       <c r="I8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2837,10 +2998,10 @@
       <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="67" t="s">
+      <c r="M8" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="N8" s="68"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2863,10 +3024,10 @@
       <c r="X8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y8" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z8" s="68"/>
+      <c r="Y8" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z8" s="64"/>
       <c r="AA8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2889,20 +3050,20 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="63" t="s">
+      <c r="G9" s="69" t="s">
         <v>236</v>
       </c>
-      <c r="H9" s="64"/>
+      <c r="H9" s="70"/>
       <c r="I9" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
-      <c r="M9" s="63" t="s">
+      <c r="M9" s="69" t="s">
         <v>222</v>
       </c>
-      <c r="N9" s="64"/>
+      <c r="N9" s="70"/>
       <c r="O9" s="11" t="s">
         <v>20</v>
       </c>
@@ -2921,10 +3082,10 @@
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
-      <c r="Y9" s="67" t="s">
+      <c r="Y9" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="Z9" s="68"/>
+      <c r="Z9" s="64"/>
       <c r="AA9" s="24" t="s">
         <v>20</v>
       </c>
@@ -2945,20 +3106,20 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="63" t="s">
+      <c r="G10" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="H10" s="64"/>
+      <c r="H10" s="70"/>
       <c r="I10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
-      <c r="M10" s="63" t="s">
+      <c r="M10" s="69" t="s">
         <v>223</v>
       </c>
-      <c r="N10" s="64"/>
+      <c r="N10" s="70"/>
       <c r="O10" s="11" t="s">
         <v>20</v>
       </c>
@@ -2977,10 +3138,10 @@
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
-      <c r="Y10" s="67" t="s">
+      <c r="Y10" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="Z10" s="68"/>
+      <c r="Z10" s="64"/>
       <c r="AA10" s="11" t="s">
         <v>21</v>
       </c>
@@ -3001,20 +3162,20 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="68"/>
+      <c r="G11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="64"/>
       <c r="I11" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="63" t="s">
+      <c r="M11" s="69" t="s">
         <v>224</v>
       </c>
-      <c r="N11" s="64"/>
+      <c r="N11" s="70"/>
       <c r="O11" s="11" t="s">
         <v>20</v>
       </c>
@@ -3033,10 +3194,10 @@
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
-      <c r="Y11" s="67" t="s">
+      <c r="Y11" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="Z11" s="68"/>
+      <c r="Z11" s="64"/>
       <c r="AA11" s="11" t="s">
         <v>20</v>
       </c>
@@ -3057,20 +3218,20 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="68"/>
+      <c r="G12" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="64"/>
       <c r="I12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
-      <c r="M12" s="63" t="s">
+      <c r="M12" s="69" t="s">
         <v>221</v>
       </c>
-      <c r="N12" s="64"/>
+      <c r="N12" s="70"/>
       <c r="O12" s="11" t="s">
         <v>20</v>
       </c>
@@ -3089,10 +3250,10 @@
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
-      <c r="Y12" s="67" t="s">
+      <c r="Y12" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="Z12" s="68"/>
+      <c r="Z12" s="64"/>
       <c r="AA12" s="11" t="s">
         <v>21</v>
       </c>
@@ -3125,10 +3286,10 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
-      <c r="M13" s="63" t="s">
+      <c r="M13" s="69" t="s">
         <v>220</v>
       </c>
-      <c r="N13" s="64"/>
+      <c r="N13" s="70"/>
       <c r="O13" s="11" t="s">
         <v>20</v>
       </c>
@@ -3147,10 +3308,10 @@
       <c r="V13" s="4"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
-      <c r="Y13" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z13" s="68"/>
+      <c r="Y13" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z13" s="64"/>
       <c r="AA13" s="11" t="s">
         <v>20</v>
       </c>
@@ -3233,20 +3394,20 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="78" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="79"/>
+      <c r="G15" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="72"/>
       <c r="I15" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="63" t="s">
+      <c r="M15" s="69" t="s">
         <v>225</v>
       </c>
-      <c r="N15" s="64"/>
+      <c r="N15" s="70"/>
       <c r="O15" s="11" t="s">
         <v>20</v>
       </c>
@@ -3265,10 +3426,10 @@
       <c r="V15" s="4"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
-      <c r="Y15" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z15" s="68"/>
+      <c r="Y15" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z15" s="64"/>
       <c r="AA15" s="11" t="s">
         <v>20</v>
       </c>
@@ -3351,20 +3512,20 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="67" t="s">
+      <c r="G17" s="63" t="s">
         <v>228</v>
       </c>
-      <c r="H17" s="68"/>
+      <c r="H17" s="64"/>
       <c r="I17" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="72" t="s">
+      <c r="M17" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="N17" s="73"/>
+      <c r="N17" s="68"/>
       <c r="O17" s="11" t="s">
         <v>19</v>
       </c>
@@ -3383,10 +3544,10 @@
       <c r="V17" s="4"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
-      <c r="Y17" s="67" t="s">
+      <c r="Y17" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="Z17" s="68"/>
+      <c r="Z17" s="64"/>
       <c r="AA17" s="24" t="s">
         <v>20</v>
       </c>
@@ -3407,40 +3568,40 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="67" t="s">
+      <c r="G18" s="63" t="s">
         <v>229</v>
       </c>
-      <c r="H18" s="68"/>
+      <c r="H18" s="64"/>
       <c r="I18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="72" t="s">
+      <c r="M18" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="N18" s="73"/>
+      <c r="N18" s="68"/>
       <c r="O18" s="11" t="s">
         <v>19</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="67" t="s">
+      <c r="S18" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="T18" s="68"/>
+      <c r="T18" s="64"/>
       <c r="U18" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
       <c r="X18" s="4"/>
-      <c r="Y18" s="67" t="s">
+      <c r="Y18" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="Z18" s="68"/>
+      <c r="Z18" s="64"/>
       <c r="AA18" s="24" t="s">
         <v>20</v>
       </c>
@@ -3461,40 +3622,40 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="67" t="s">
+      <c r="G19" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="H19" s="68"/>
+      <c r="H19" s="64"/>
       <c r="I19" s="11" t="s">
         <v>21</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
-      <c r="M19" s="72" t="s">
+      <c r="M19" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="N19" s="73"/>
+      <c r="N19" s="68"/>
       <c r="O19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="72" t="s">
+      <c r="S19" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="T19" s="73"/>
+      <c r="T19" s="68"/>
       <c r="U19" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V19" s="4"/>
       <c r="W19" s="4"/>
       <c r="X19" s="4"/>
-      <c r="Y19" s="67" t="s">
+      <c r="Y19" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="Z19" s="68"/>
+      <c r="Z19" s="64"/>
       <c r="AA19" s="24" t="s">
         <v>20</v>
       </c>
@@ -3515,40 +3676,40 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="63" t="s">
         <v>231</v>
       </c>
-      <c r="H20" s="68"/>
+      <c r="H20" s="64"/>
       <c r="I20" s="11" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="67" t="s">
+      <c r="M20" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="N20" s="68"/>
+      <c r="N20" s="64"/>
       <c r="O20" s="11" t="s">
         <v>20</v>
       </c>
       <c r="P20" s="4"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="67" t="s">
+      <c r="S20" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="T20" s="68"/>
+      <c r="T20" s="64"/>
       <c r="U20" s="24" t="s">
         <v>20</v>
       </c>
       <c r="V20" s="4"/>
       <c r="W20" s="4"/>
       <c r="X20" s="4"/>
-      <c r="Y20" s="67" t="s">
+      <c r="Y20" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="Z20" s="68"/>
+      <c r="Z20" s="64"/>
       <c r="AA20" s="24" t="s">
         <v>20</v>
       </c>
@@ -3575,10 +3736,10 @@
       <c r="F21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="67" t="s">
+      <c r="G21" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="H21" s="68"/>
+      <c r="H21" s="64"/>
       <c r="I21" s="11" t="s">
         <v>19</v>
       </c>
@@ -3627,10 +3788,10 @@
       <c r="X21" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y21" s="67" t="s">
+      <c r="Y21" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="Z21" s="68"/>
+      <c r="Z21" s="64"/>
       <c r="AA21" s="24" t="s">
         <v>21</v>
       </c>
@@ -3663,10 +3824,10 @@
       <c r="F22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="67" t="s">
+      <c r="G22" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="68"/>
+      <c r="H22" s="64"/>
       <c r="I22" s="11" t="s">
         <v>19</v>
       </c>
@@ -3715,10 +3876,10 @@
       <c r="X22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y22" s="67" t="s">
+      <c r="Y22" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="Z22" s="68"/>
+      <c r="Z22" s="64"/>
       <c r="AA22" s="24" t="s">
         <v>21</v>
       </c>
@@ -3751,10 +3912,10 @@
       <c r="F23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="67" t="s">
+      <c r="G23" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="H23" s="68"/>
+      <c r="H23" s="64"/>
       <c r="I23" s="11" t="s">
         <v>21</v>
       </c>
@@ -3791,10 +3952,10 @@
       <c r="X23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y23" s="67" t="s">
+      <c r="Y23" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="Z23" s="68"/>
+      <c r="Z23" s="64"/>
       <c r="AA23" s="24" t="s">
         <v>21</v>
       </c>
@@ -3827,10 +3988,10 @@
       <c r="F24" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="67" t="s">
+      <c r="G24" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="68"/>
+      <c r="H24" s="64"/>
       <c r="I24" s="11" t="s">
         <v>21</v>
       </c>
@@ -3869,10 +4030,10 @@
       <c r="X24" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y24" s="67" t="s">
+      <c r="Y24" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="Z24" s="68"/>
+      <c r="Z24" s="64"/>
       <c r="AA24" s="24" t="s">
         <v>21</v>
       </c>
@@ -3905,10 +4066,10 @@
       <c r="F25" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="68"/>
+      <c r="G25" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="64"/>
       <c r="I25" s="23" t="s">
         <v>21</v>
       </c>
@@ -3955,10 +4116,10 @@
       <c r="X25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Y25" s="67" t="s">
+      <c r="Y25" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="Z25" s="68"/>
+      <c r="Z25" s="64"/>
       <c r="AA25" s="25" t="s">
         <v>21</v>
       </c>
@@ -3991,10 +4152,10 @@
       <c r="F26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="68"/>
+      <c r="G26" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="64"/>
       <c r="I26" s="11" t="s">
         <v>21</v>
       </c>
@@ -4043,10 +4204,10 @@
       <c r="X26" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y26" s="67" t="s">
+      <c r="Y26" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="Z26" s="68"/>
+      <c r="Z26" s="64"/>
       <c r="AA26" s="24" t="s">
         <v>21</v>
       </c>
@@ -4079,10 +4240,10 @@
       <c r="F27" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G27" s="67" t="s">
+      <c r="G27" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="68"/>
+      <c r="H27" s="64"/>
       <c r="I27" s="11" t="s">
         <v>21</v>
       </c>
@@ -4131,10 +4292,10 @@
       <c r="X27" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y27" s="67" t="s">
+      <c r="Y27" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="Z27" s="68"/>
+      <c r="Z27" s="64"/>
       <c r="AA27" s="24" t="s">
         <v>21</v>
       </c>
@@ -4167,10 +4328,10 @@
       <c r="F28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="67" t="s">
+      <c r="G28" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="H28" s="68"/>
+      <c r="H28" s="64"/>
       <c r="I28" s="11" t="s">
         <v>21</v>
       </c>
@@ -4219,10 +4380,10 @@
       <c r="X28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y28" s="67" t="s">
+      <c r="Y28" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="Z28" s="68"/>
+      <c r="Z28" s="64"/>
       <c r="AA28" s="24" t="s">
         <v>21</v>
       </c>
@@ -4255,10 +4416,10 @@
       <c r="F29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="67" t="s">
+      <c r="G29" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="68"/>
+      <c r="H29" s="64"/>
       <c r="I29" s="11" t="s">
         <v>21</v>
       </c>
@@ -4305,10 +4466,10 @@
       <c r="X29" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y29" s="67" t="s">
+      <c r="Y29" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="Z29" s="68"/>
+      <c r="Z29" s="64"/>
       <c r="AA29" s="24" t="s">
         <v>21</v>
       </c>
@@ -4341,10 +4502,10 @@
       <c r="F30" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="67" t="s">
+      <c r="G30" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="H30" s="68"/>
+      <c r="H30" s="64"/>
       <c r="I30" s="11" t="s">
         <v>21</v>
       </c>
@@ -4393,10 +4554,10 @@
       <c r="X30" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y30" s="67" t="s">
+      <c r="Y30" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="68"/>
+      <c r="Z30" s="64"/>
       <c r="AA30" s="24" t="s">
         <v>21</v>
       </c>
@@ -4429,10 +4590,10 @@
       <c r="F31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="67" t="s">
+      <c r="G31" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="68"/>
+      <c r="H31" s="64"/>
       <c r="I31" s="11" t="s">
         <v>21</v>
       </c>
@@ -4481,10 +4642,10 @@
       <c r="X31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y31" s="67" t="s">
+      <c r="Y31" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="Z31" s="68"/>
+      <c r="Z31" s="64"/>
       <c r="AA31" s="24" t="s">
         <v>21</v>
       </c>
@@ -4517,10 +4678,10 @@
       <c r="F32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G32" s="67" t="s">
+      <c r="G32" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="H32" s="68"/>
+      <c r="H32" s="64"/>
       <c r="I32" s="11" t="s">
         <v>21</v>
       </c>
@@ -4569,10 +4730,10 @@
       <c r="X32" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y32" s="67" t="s">
+      <c r="Y32" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="Z32" s="68"/>
+      <c r="Z32" s="64"/>
       <c r="AA32" s="24" t="s">
         <v>21</v>
       </c>
@@ -4605,10 +4766,10 @@
       <c r="F33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="67" t="s">
+      <c r="G33" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="68"/>
+      <c r="H33" s="64"/>
       <c r="I33" s="11" t="s">
         <v>21</v>
       </c>
@@ -4655,10 +4816,10 @@
       <c r="X33" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y33" s="67" t="s">
+      <c r="Y33" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="Z33" s="68"/>
+      <c r="Z33" s="64"/>
       <c r="AA33" s="24" t="s">
         <v>21</v>
       </c>
@@ -4691,10 +4852,10 @@
       <c r="F34" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="67" t="s">
+      <c r="G34" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="68"/>
+      <c r="H34" s="64"/>
       <c r="I34" s="11" t="s">
         <v>21</v>
       </c>
@@ -4743,10 +4904,10 @@
       <c r="X34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y34" s="67" t="s">
+      <c r="Y34" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="Z34" s="68"/>
+      <c r="Z34" s="64"/>
       <c r="AA34" s="24" t="s">
         <v>21</v>
       </c>
@@ -4775,10 +4936,10 @@
       <c r="F35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="67" t="s">
+      <c r="G35" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="H35" s="68"/>
+      <c r="H35" s="64"/>
       <c r="I35" s="24" t="s">
         <v>21</v>
       </c>
@@ -4787,10 +4948,10 @@
       <c r="L35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M35" s="67" t="s">
+      <c r="M35" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="N35" s="68"/>
+      <c r="N35" s="64"/>
       <c r="O35" s="24" t="s">
         <v>21</v>
       </c>
@@ -4811,10 +4972,10 @@
       <c r="X35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Y35" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z35" s="68"/>
+      <c r="Y35" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z35" s="64"/>
       <c r="AA35" s="11"/>
       <c r="AB35" s="4"/>
       <c r="AC35" s="4"/>
@@ -4837,10 +4998,10 @@
       <c r="F36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="76" t="s">
+      <c r="G36" s="65" t="s">
         <v>160</v>
       </c>
-      <c r="H36" s="77"/>
+      <c r="H36" s="66"/>
       <c r="I36" s="26" t="s">
         <v>20</v>
       </c>
@@ -4849,10 +5010,10 @@
       <c r="L36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M36" s="76" t="s">
+      <c r="M36" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="N36" s="77"/>
+      <c r="N36" s="66"/>
       <c r="O36" s="26" t="s">
         <v>20</v>
       </c>
@@ -4873,10 +5034,10 @@
       <c r="X36" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Y36" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z36" s="77"/>
+      <c r="Y36" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z36" s="66"/>
       <c r="AA36" s="12"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="13"/>
@@ -5011,10 +5172,10 @@
       <c r="L39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M39" s="74" t="s">
+      <c r="M39" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="N39" s="75"/>
+      <c r="N39" s="74"/>
       <c r="O39" s="24" t="s">
         <v>21</v>
       </c>
@@ -5095,10 +5256,10 @@
       <c r="L40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="M40" s="74" t="s">
+      <c r="M40" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="N40" s="75"/>
+      <c r="N40" s="74"/>
       <c r="O40" s="24" t="s">
         <v>21</v>
       </c>
@@ -5648,27 +5809,27 @@
       <c r="AD48" s="13"/>
       <c r="AE48" s="15"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:23">
       <c r="A49" s="1"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:23">
       <c r="B51" s="38"/>
       <c r="H51" s="2"/>
       <c r="K51" s="38"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:23">
       <c r="B52" s="37"/>
       <c r="M52" s="38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:23">
       <c r="B53" s="37"/>
       <c r="H53" s="2"/>
       <c r="K53" s="37"/>
       <c r="M53" s="38"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:23">
       <c r="B54" s="37"/>
       <c r="H54" s="2"/>
       <c r="K54" s="37"/>
@@ -5676,7 +5837,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:23">
       <c r="B55" s="37"/>
       <c r="H55" s="2"/>
       <c r="K55" s="37"/>
@@ -5684,7 +5845,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:23">
       <c r="B56" s="37"/>
       <c r="H56" s="2"/>
       <c r="K56" s="37"/>
@@ -5692,7 +5853,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:23">
       <c r="B57" s="37"/>
       <c r="H57" s="2"/>
       <c r="K57" s="37"/>
@@ -5700,181 +5861,336 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:23" ht="15.75" thickBot="1">
       <c r="B58" s="37"/>
       <c r="H58" s="38"/>
       <c r="K58" s="37"/>
       <c r="M58" s="44" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="P58" s="83" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q58" s="83"/>
+      <c r="R58" s="83"/>
+      <c r="S58" s="83"/>
+      <c r="T58" s="83"/>
+      <c r="U58" s="83"/>
+      <c r="V58" s="83"/>
+      <c r="W58" s="83"/>
+    </row>
+    <row r="59" spans="1:23" ht="15.75" thickBot="1">
       <c r="B59" s="1"/>
       <c r="H59" s="2"/>
       <c r="K59" s="37"/>
       <c r="M59" s="44" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="P59" s="84" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q59" s="85"/>
+      <c r="R59" s="85"/>
+      <c r="S59" s="86" t="s">
+        <v>240</v>
+      </c>
+      <c r="T59" s="87" t="s">
+        <v>241</v>
+      </c>
+      <c r="U59" s="87"/>
+      <c r="V59" s="87"/>
+      <c r="W59" s="88"/>
+    </row>
+    <row r="60" spans="1:23">
       <c r="B60" s="1"/>
       <c r="H60" s="2"/>
       <c r="K60" s="37"/>
       <c r="M60" s="44" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="P60" s="89" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q60" s="90"/>
+      <c r="R60" s="90"/>
+      <c r="S60" s="91" t="s">
+        <v>260</v>
+      </c>
+      <c r="T60" s="92" t="s">
+        <v>243</v>
+      </c>
+      <c r="U60" s="92"/>
+      <c r="V60" s="92"/>
+      <c r="W60" s="93"/>
+    </row>
+    <row r="61" spans="1:23">
       <c r="H61" s="2"/>
       <c r="K61" s="37"/>
       <c r="M61" s="38"/>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="P61" s="94" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q61" s="95"/>
+      <c r="R61" s="95"/>
+      <c r="S61" s="96" t="s">
+        <v>259</v>
+      </c>
+      <c r="T61" s="97" t="s">
+        <v>245</v>
+      </c>
+      <c r="U61" s="97"/>
+      <c r="V61" s="97"/>
+      <c r="W61" s="98"/>
+    </row>
+    <row r="62" spans="1:23">
       <c r="B62" s="37"/>
       <c r="H62" s="2"/>
       <c r="M62" s="38"/>
-      <c r="P62" s="37"/>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="P62" s="94" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q62" s="95"/>
+      <c r="R62" s="95"/>
+      <c r="S62" s="96" t="s">
+        <v>247</v>
+      </c>
+      <c r="T62" s="97" t="s">
+        <v>248</v>
+      </c>
+      <c r="U62" s="97"/>
+      <c r="V62" s="97"/>
+      <c r="W62" s="98"/>
+    </row>
+    <row r="63" spans="1:23">
       <c r="H63" s="2"/>
       <c r="M63" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="P63" s="37"/>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="P63" s="94" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q63" s="95"/>
+      <c r="R63" s="95"/>
+      <c r="S63" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="T63" s="97" t="s">
+        <v>251</v>
+      </c>
+      <c r="U63" s="97"/>
+      <c r="V63" s="97"/>
+      <c r="W63" s="98"/>
+    </row>
+    <row r="64" spans="1:23">
       <c r="B64" s="38"/>
       <c r="H64" s="2"/>
       <c r="K64" s="38"/>
       <c r="M64" s="44" t="s">
         <v>174</v>
       </c>
-      <c r="P64" s="37"/>
-    </row>
-    <row r="65" spans="2:16">
+      <c r="P64" s="94" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q64" s="95"/>
+      <c r="R64" s="95"/>
+      <c r="S64" s="96" t="s">
+        <v>253</v>
+      </c>
+      <c r="T64" s="97" t="s">
+        <v>254</v>
+      </c>
+      <c r="U64" s="97"/>
+      <c r="V64" s="97"/>
+      <c r="W64" s="98"/>
+    </row>
+    <row r="65" spans="2:23">
       <c r="B65" s="37"/>
       <c r="H65" s="2"/>
       <c r="M65" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="P65" s="37"/>
-    </row>
-    <row r="66" spans="2:16">
+      <c r="P65" s="94" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q65" s="95"/>
+      <c r="R65" s="95"/>
+      <c r="S65" s="96" t="s">
+        <v>256</v>
+      </c>
+      <c r="T65" s="99"/>
+      <c r="U65" s="99"/>
+      <c r="V65" s="99"/>
+      <c r="W65" s="100"/>
+    </row>
+    <row r="66" spans="2:23" ht="15.75" thickBot="1">
       <c r="B66" s="37"/>
       <c r="H66" s="2"/>
       <c r="K66" s="37"/>
-      <c r="P66" s="37"/>
-    </row>
-    <row r="67" spans="2:16">
+      <c r="P66" s="101" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q66" s="102"/>
+      <c r="R66" s="102"/>
+      <c r="S66" s="103" t="s">
+        <v>258</v>
+      </c>
+      <c r="T66" s="104"/>
+      <c r="U66" s="104"/>
+      <c r="V66" s="104"/>
+      <c r="W66" s="105"/>
+    </row>
+    <row r="67" spans="2:23">
       <c r="B67" s="37"/>
       <c r="H67" s="2"/>
       <c r="K67" s="37"/>
       <c r="P67" s="37"/>
     </row>
-    <row r="68" spans="2:16">
+    <row r="68" spans="2:23">
       <c r="B68" s="37"/>
       <c r="H68" s="2"/>
       <c r="K68" s="37"/>
       <c r="P68" s="37"/>
     </row>
-    <row r="69" spans="2:16">
+    <row r="69" spans="2:23">
       <c r="B69" s="37"/>
       <c r="H69" s="37"/>
       <c r="K69" s="37"/>
       <c r="P69" s="37"/>
     </row>
-    <row r="70" spans="2:16">
+    <row r="70" spans="2:23">
       <c r="H70" s="37"/>
       <c r="P70" s="37"/>
     </row>
-    <row r="71" spans="2:16">
+    <row r="71" spans="2:23">
       <c r="B71" s="38"/>
       <c r="H71" s="37"/>
       <c r="P71" s="37"/>
     </row>
-    <row r="72" spans="2:16">
+    <row r="72" spans="2:23">
       <c r="B72" s="38"/>
       <c r="H72" s="37"/>
       <c r="P72" s="37"/>
     </row>
-    <row r="73" spans="2:16">
+    <row r="73" spans="2:23">
       <c r="B73" s="38"/>
       <c r="H73" s="37"/>
       <c r="P73" s="37"/>
     </row>
-    <row r="74" spans="2:16">
+    <row r="74" spans="2:23">
       <c r="B74" s="38"/>
       <c r="H74" s="37"/>
       <c r="P74" s="37"/>
     </row>
-    <row r="75" spans="2:16">
+    <row r="75" spans="2:23">
       <c r="H75" s="37"/>
       <c r="P75" s="37"/>
     </row>
-    <row r="76" spans="2:16">
+    <row r="76" spans="2:23">
       <c r="H76" s="37"/>
       <c r="P76" s="37"/>
     </row>
-    <row r="77" spans="2:16">
+    <row r="77" spans="2:23">
       <c r="H77" s="37"/>
       <c r="P77" s="37"/>
     </row>
-    <row r="78" spans="2:16">
+    <row r="78" spans="2:23">
       <c r="H78" s="37"/>
       <c r="P78" s="37"/>
     </row>
-    <row r="79" spans="2:16">
+    <row r="79" spans="2:23">
       <c r="H79" s="37"/>
       <c r="P79" s="37"/>
     </row>
-    <row r="80" spans="2:16">
+    <row r="80" spans="2:23">
       <c r="H80" s="37"/>
       <c r="P80" s="37"/>
     </row>
-    <row r="81" spans="2:8">
+    <row r="81" spans="2:16">
       <c r="H81" s="37"/>
-    </row>
-    <row r="89" spans="2:8">
+      <c r="P81" s="37"/>
+    </row>
+    <row r="89" spans="2:16">
       <c r="B89" s="38"/>
     </row>
-    <row r="90" spans="2:8">
+    <row r="90" spans="2:16">
       <c r="B90" s="38"/>
     </row>
-    <row r="91" spans="2:8">
+    <row r="91" spans="2:16">
       <c r="B91" s="38"/>
     </row>
-    <row r="92" spans="2:8">
+    <row r="92" spans="2:16">
       <c r="B92" s="38"/>
     </row>
-    <row r="93" spans="2:8">
+    <row r="93" spans="2:16">
       <c r="B93" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="88">
-    <mergeCell ref="Y22:Z22"/>
-    <mergeCell ref="Y21:Z21"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="Y8:Z8"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y10:Z10"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y7:Z7"/>
-    <mergeCell ref="Y36:Z36"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="Y35:Z35"/>
+  <mergeCells count="105">
+    <mergeCell ref="P58:W58"/>
+    <mergeCell ref="T59:W59"/>
+    <mergeCell ref="T66:W66"/>
+    <mergeCell ref="T65:W65"/>
+    <mergeCell ref="T64:W64"/>
+    <mergeCell ref="T63:W63"/>
+    <mergeCell ref="T62:W62"/>
+    <mergeCell ref="T61:W61"/>
+    <mergeCell ref="P64:R64"/>
+    <mergeCell ref="P65:R65"/>
+    <mergeCell ref="P66:R66"/>
+    <mergeCell ref="T60:W60"/>
+    <mergeCell ref="P59:R59"/>
+    <mergeCell ref="P60:R60"/>
+    <mergeCell ref="P61:R61"/>
+    <mergeCell ref="P62:R62"/>
+    <mergeCell ref="P63:R63"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="U2:Z2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="Y15:Z15"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G26:H26"/>
@@ -5891,54 +6207,30 @@
     <mergeCell ref="Y17:Z17"/>
     <mergeCell ref="Y24:Z24"/>
     <mergeCell ref="Y23:Z23"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="M40:N40"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="U2:Z2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="Y36:Z36"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="Y30:Z30"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="Y8:Z8"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y10:Z10"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y7:Z7"/>
+    <mergeCell ref="Y22:Z22"/>
+    <mergeCell ref="Y21:Z21"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y25:Z25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5990,41 +6282,41 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="69" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="69" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="69" t="s">
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="69" t="s">
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="75" t="s">
         <v>122</v>
       </c>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="71"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="76"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="77"/>
     </row>
     <row r="3" spans="2:27" ht="15.75" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -8340,27 +8632,27 @@
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="69" t="s">
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="69" t="s">
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="71"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="77"/>
       <c r="R2" s="80" t="s">
         <v>4</v>
       </c>

</xml_diff>